<commit_message>
:art: duplicate game analyze class
</commit_message>
<xml_diff>
--- a/turns_statistics.xlsx
+++ b/turns_statistics.xlsx
@@ -444,7 +444,7 @@
         <v>1200</v>
       </c>
       <c r="D3">
-        <v>124.6160625703799</v>
+        <v>124.60358675391</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -455,10 +455,10 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>6150</v>
+        <v>5850</v>
       </c>
       <c r="D4">
-        <v>435.35095</v>
+        <v>435.97225</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -472,7 +472,7 @@
         <v>32</v>
       </c>
       <c r="D5">
-        <v>3.493538</v>
+        <v>3.498874</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -483,10 +483,10 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6">
-        <v>0.4474103330205654</v>
+        <v>0.4497412596166652</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -500,7 +500,7 @@
         <v>8</v>
       </c>
       <c r="D7">
-        <v>0.337318</v>
+        <v>0.338133</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -514,7 +514,7 @@
         <v>5</v>
       </c>
       <c r="D8">
-        <v>2.174218</v>
+        <v>2.173811</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -528,7 +528,7 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <v>3.344364080196065</v>
+        <v>3.34426818456452</v>
       </c>
     </row>
   </sheetData>

</xml_diff>